<commit_message>
Connor: Added the basics for an Electron Client Application and updated the GanttChart.xlsx
</commit_message>
<xml_diff>
--- a/Documentation/GanttChart.xlsx
+++ b/Documentation/GanttChart.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>TASK</t>
   </si>
@@ -38,9 +38,6 @@
     <t>END DATE</t>
   </si>
   <si>
-    <t>Design Client Program UI</t>
-  </si>
-  <si>
     <t>Setup infrastructure to allow for deployment of applications</t>
   </si>
   <si>
@@ -50,18 +47,12 @@
     <t>Buy and assemble componenets of the System</t>
   </si>
   <si>
-    <t>Process web requests in the Edge Cluster</t>
-  </si>
-  <si>
     <t>Update Edge Server program to return web response</t>
   </si>
   <si>
     <t>Update Client Program to handle responses</t>
   </si>
   <si>
-    <t>Update Client Program to match design</t>
-  </si>
-  <si>
     <t>Update Client Program to make multiple web requests</t>
   </si>
   <si>
@@ -86,15 +77,6 @@
     <t>Perform analysis and update machine learning application</t>
   </si>
   <si>
-    <t>Create Basic Client program to make web requests</t>
-  </si>
-  <si>
-    <t>Create Edge Server program to receive web requests</t>
-  </si>
-  <si>
-    <t>Create Data Centre program to receive web requests</t>
-  </si>
-  <si>
     <t>Update Data Centre program to process web requests</t>
   </si>
   <si>
@@ -102,6 +84,30 @@
   </si>
   <si>
     <t xml:space="preserve">Research and design caching application </t>
+  </si>
+  <si>
+    <t>Create Basic Edge Server Program</t>
+  </si>
+  <si>
+    <t>Create Data Centre program</t>
+  </si>
+  <si>
+    <t>Update Basic Client program to make web requests</t>
+  </si>
+  <si>
+    <t>Create Basic Client Program</t>
+  </si>
+  <si>
+    <t>Update Client Program Design</t>
+  </si>
+  <si>
+    <t>Update Data Centre Program to receive web requests</t>
+  </si>
+  <si>
+    <t>Update Edge Server Program to receive web requests</t>
+  </si>
+  <si>
+    <t>Update Edge Server Program to process web requests</t>
   </si>
 </sst>
 </file>
@@ -207,9 +213,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Gantt Chart'!$A$2:$A$23</c:f>
+              <c:f>'Gantt Chart'!$A$2:$A$29</c:f>
               <c:strCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>Buy and assemble componenets of the System</c:v>
                 </c:pt>
@@ -217,63 +223,69 @@
                   <c:v>Setup infrastructure to allow for deployment of applications</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Create Basic Client program to make web requests</c:v>
+                  <c:v>Create Basic Client Program</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Create Edge Server program to receive web requests</c:v>
+                  <c:v>Update Basic Client program to make web requests</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Create Data Centre program to receive web requests</c:v>
+                  <c:v>Create Basic Edge Server Program</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Update Edge Server program to return web response</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Create Data Centre program</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Update Data Centre program to return web responses</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Update Client Program Design</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Update Edge Server Program to receive web requests</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Update Edge Server Program to process web requests</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Update Data Centre Program to receive web requests</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Update Data Centre program to process web requests</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>Update Data Centre program to return web responses</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Process web requests in the Edge Cluster</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Update Edge Server program to return web response</c:v>
-                </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
                   <c:v>Update Client Program to handle responses</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>Design Client Program UI</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Update Client Program to match design</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>Update Client Program to make multiple web requests</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="19">
                   <c:v>Research and design caching application </c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="20">
                   <c:v>Create image for the cachine application</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="21">
                   <c:v>Perform analysis and update caching application</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="22">
                   <c:v>Research and design voice recognition application</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="23">
                   <c:v>Create image for voice recognition application</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="24">
                   <c:v>Perform analysis and update voice recognition application</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="25">
                   <c:v>Research and design machine learning application</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="26">
                   <c:v>Create image for machine learning application</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="27">
                   <c:v>Perform analysis and update machine learning application</c:v>
                 </c:pt>
               </c:strCache>
@@ -386,9 +398,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Gantt Chart'!$A$2:$A$23</c:f>
+              <c:f>'Gantt Chart'!$A$2:$A$29</c:f>
               <c:strCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>Buy and assemble componenets of the System</c:v>
                 </c:pt>
@@ -396,63 +408,69 @@
                   <c:v>Setup infrastructure to allow for deployment of applications</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Create Basic Client program to make web requests</c:v>
+                  <c:v>Create Basic Client Program</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Create Edge Server program to receive web requests</c:v>
+                  <c:v>Update Basic Client program to make web requests</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Create Data Centre program to receive web requests</c:v>
+                  <c:v>Create Basic Edge Server Program</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Update Edge Server program to return web response</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Create Data Centre program</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Update Data Centre program to return web responses</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Update Client Program Design</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Update Edge Server Program to receive web requests</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Update Edge Server Program to process web requests</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Update Data Centre Program to receive web requests</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Update Data Centre program to process web requests</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>Update Data Centre program to return web responses</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Process web requests in the Edge Cluster</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Update Edge Server program to return web response</c:v>
-                </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
                   <c:v>Update Client Program to handle responses</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>Design Client Program UI</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Update Client Program to match design</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>Update Client Program to make multiple web requests</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="19">
                   <c:v>Research and design caching application </c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="20">
                   <c:v>Create image for the cachine application</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="21">
                   <c:v>Perform analysis and update caching application</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="22">
                   <c:v>Research and design voice recognition application</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="23">
                   <c:v>Create image for voice recognition application</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="24">
                   <c:v>Perform analysis and update voice recognition application</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="25">
                   <c:v>Research and design machine learning application</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="26">
                   <c:v>Create image for machine learning application</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="27">
                   <c:v>Perform analysis and update machine learning application</c:v>
                 </c:pt>
               </c:strCache>
@@ -1589,10 +1607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1617,7 +1635,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2">
         <v>42654</v>
@@ -1632,7 +1650,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2">
         <f>D2</f>
@@ -1648,7 +1666,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2">
         <f t="shared" ref="B4:B23" si="1">D3</f>
@@ -1664,7 +1682,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" si="1"/>
@@ -1680,7 +1698,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" si="1"/>
@@ -1696,7 +1714,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2">
         <f t="shared" si="1"/>
@@ -1712,7 +1730,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" si="1"/>
@@ -1728,7 +1746,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" si="1"/>
@@ -1744,7 +1762,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" si="1"/>
@@ -1760,7 +1778,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" si="1"/>
@@ -1776,7 +1794,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" si="1"/>
@@ -1792,7 +1810,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" si="1"/>
@@ -1808,7 +1826,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" si="1"/>
@@ -1824,7 +1842,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" si="1"/>
@@ -1840,7 +1858,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" si="1"/>
@@ -1855,9 +1873,6 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
       <c r="B17" s="2">
         <f t="shared" si="1"/>
         <v>42731</v>
@@ -1871,9 +1886,6 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
       <c r="B18" s="2">
         <f t="shared" si="1"/>
         <v>42747</v>
@@ -1887,9 +1899,6 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
       <c r="B19" s="2">
         <f t="shared" si="1"/>
         <v>42752</v>
@@ -1903,9 +1912,6 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
       <c r="B20" s="2">
         <f t="shared" si="1"/>
         <v>42766</v>
@@ -1920,7 +1926,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2">
         <f t="shared" si="1"/>
@@ -1936,7 +1942,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B22" s="2">
         <f t="shared" si="1"/>
@@ -1952,7 +1958,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B23" s="2">
         <f t="shared" si="1"/>
@@ -1964,6 +1970,36 @@
       <c r="D23" s="1">
         <f t="shared" si="0"/>
         <v>42808</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Connor: Updated with work completed over the weekend. This includes an updated document with better references and better verifiable criteria. Also did inital commit of EdgeNode docker information as I have a basic version of it working. I have tried to add references to everything that helped me to get up and running but I will need to make sure this is the case.
</commit_message>
<xml_diff>
--- a/Documentation/GanttChart.xlsx
+++ b/Documentation/GanttChart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\condl\Dropbox\ComputerScienceYearFour\CSC3002-CS Project\ProjectDocuments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SourceControl\FinalYearProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>TASK</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Buy and assemble componenets of the System</t>
   </si>
   <si>
-    <t>Update Edge Server program to return web response</t>
-  </si>
-  <si>
     <t>Update Client Program to handle responses</t>
   </si>
   <si>
@@ -80,24 +77,9 @@
     <t>Update Data Centre program to process web requests</t>
   </si>
   <si>
-    <t>Update Data Centre program to return web responses</t>
-  </si>
-  <si>
     <t xml:space="preserve">Research and design caching application </t>
   </si>
   <si>
-    <t>Create Basic Edge Server Program</t>
-  </si>
-  <si>
-    <t>Create Data Centre program</t>
-  </si>
-  <si>
-    <t>Update Basic Client program to make web requests</t>
-  </si>
-  <si>
-    <t>Create Basic Client Program</t>
-  </si>
-  <si>
     <t>Update Client Program Design</t>
   </si>
   <si>
@@ -108,6 +90,15 @@
   </si>
   <si>
     <t>Update Edge Server Program to process web requests</t>
+  </si>
+  <si>
+    <t>Create Basic Client Program to make web requests</t>
+  </si>
+  <si>
+    <t>Create Basic Edge Server Program to return web response</t>
+  </si>
+  <si>
+    <t>Create Data Centre program to return web responses</t>
   </si>
 </sst>
 </file>
@@ -213,9 +204,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Gantt Chart'!$A$2:$A$29</c:f>
+              <c:f>'Gantt Chart'!$A$2:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="28"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>Buy and assemble componenets of the System</c:v>
                 </c:pt>
@@ -223,69 +214,60 @@
                   <c:v>Setup infrastructure to allow for deployment of applications</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Create Basic Client Program</c:v>
+                  <c:v>Create Basic Client Program to make web requests</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Update Basic Client program to make web requests</c:v>
+                  <c:v>Create Basic Edge Server Program to return web response</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Create Basic Edge Server Program</c:v>
+                  <c:v>Create Data Centre program to return web responses</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Update Edge Server program to return web response</c:v>
+                  <c:v>Update Client Program Design</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Create Data Centre program</c:v>
+                  <c:v>Update Edge Server Program to receive web requests</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Update Data Centre program to return web responses</c:v>
+                  <c:v>Update Edge Server Program to process web requests</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Update Client Program Design</c:v>
+                  <c:v>Update Data Centre Program to receive web requests</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Update Edge Server Program to receive web requests</c:v>
+                  <c:v>Update Data Centre program to process web requests</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Update Edge Server Program to process web requests</c:v>
+                  <c:v>Update Client Program to handle responses</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Update Data Centre Program to receive web requests</c:v>
+                  <c:v>Update Client Program to make multiple web requests</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Update Data Centre program to process web requests</c:v>
+                  <c:v>Research and design caching application </c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Update Client Program to handle responses</c:v>
+                  <c:v>Create image for the cachine application</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Update Client Program to make multiple web requests</c:v>
+                  <c:v>Perform analysis and update caching application</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Research and design voice recognition application</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Create image for voice recognition application</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Perform analysis and update voice recognition application</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Research and design machine learning application</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Research and design caching application </c:v>
+                  <c:v>Create image for machine learning application</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Create image for the cachine application</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Perform analysis and update caching application</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Research and design voice recognition application</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Create image for voice recognition application</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Perform analysis and update voice recognition application</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Research and design machine learning application</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Create image for machine learning application</c:v>
-                </c:pt>
-                <c:pt idx="27">
                   <c:v>Perform analysis and update machine learning application</c:v>
                 </c:pt>
               </c:strCache>
@@ -293,10 +275,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Gantt Chart'!$B$2:$B$23</c:f>
+              <c:f>'Gantt Chart'!$B$2:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>d/m;@</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>42654</c:v>
                 </c:pt>
@@ -359,9 +341,6 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>42780</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>42794</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -398,9 +377,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Gantt Chart'!$A$2:$A$29</c:f>
+              <c:f>'Gantt Chart'!$A$2:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="28"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>Buy and assemble componenets of the System</c:v>
                 </c:pt>
@@ -408,69 +387,60 @@
                   <c:v>Setup infrastructure to allow for deployment of applications</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Create Basic Client Program</c:v>
+                  <c:v>Create Basic Client Program to make web requests</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Update Basic Client program to make web requests</c:v>
+                  <c:v>Create Basic Edge Server Program to return web response</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Create Basic Edge Server Program</c:v>
+                  <c:v>Create Data Centre program to return web responses</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Update Edge Server program to return web response</c:v>
+                  <c:v>Update Client Program Design</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Create Data Centre program</c:v>
+                  <c:v>Update Edge Server Program to receive web requests</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Update Data Centre program to return web responses</c:v>
+                  <c:v>Update Edge Server Program to process web requests</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Update Client Program Design</c:v>
+                  <c:v>Update Data Centre Program to receive web requests</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Update Edge Server Program to receive web requests</c:v>
+                  <c:v>Update Data Centre program to process web requests</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Update Edge Server Program to process web requests</c:v>
+                  <c:v>Update Client Program to handle responses</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Update Data Centre Program to receive web requests</c:v>
+                  <c:v>Update Client Program to make multiple web requests</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Update Data Centre program to process web requests</c:v>
+                  <c:v>Research and design caching application </c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Update Client Program to handle responses</c:v>
+                  <c:v>Create image for the cachine application</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Update Client Program to make multiple web requests</c:v>
+                  <c:v>Perform analysis and update caching application</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Research and design voice recognition application</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Create image for voice recognition application</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Perform analysis and update voice recognition application</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Research and design machine learning application</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Research and design caching application </c:v>
+                  <c:v>Create image for machine learning application</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Create image for the cachine application</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Perform analysis and update caching application</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Research and design voice recognition application</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Create image for voice recognition application</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Perform analysis and update voice recognition application</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Research and design machine learning application</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Create image for machine learning application</c:v>
-                </c:pt>
-                <c:pt idx="27">
                   <c:v>Perform analysis and update machine learning application</c:v>
                 </c:pt>
               </c:strCache>
@@ -478,10 +448,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Gantt Chart'!$C$2:$C$23</c:f>
+              <c:f>'Gantt Chart'!$C$2:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -543,9 +513,6 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="21">
                   <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
@@ -1607,19 +1574,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="X30" sqref="X30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1633,7 +1600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1648,7 +1615,7 @@
         <v>42659</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1660,16 +1627,16 @@
         <v>7</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D23" si="0">B3+C3</f>
+        <f t="shared" ref="D3:D22" si="0">B3+C3</f>
         <v>42666</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2">
-        <f t="shared" ref="B4:B23" si="1">D3</f>
+        <f t="shared" ref="B4:B22" si="1">D3</f>
         <v>42666</v>
       </c>
       <c r="C4">
@@ -1680,9 +1647,9 @@
         <v>42670</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" si="1"/>
@@ -1696,9 +1663,9 @@
         <v>42676</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" si="1"/>
@@ -1712,9 +1679,9 @@
         <v>42680</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2">
         <f t="shared" si="1"/>
@@ -1728,9 +1695,9 @@
         <v>42686</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" si="1"/>
@@ -1744,9 +1711,9 @@
         <v>42688</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" si="1"/>
@@ -1760,9 +1727,9 @@
         <v>42694</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" si="1"/>
@@ -1776,9 +1743,9 @@
         <v>42699</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" si="1"/>
@@ -1792,9 +1759,9 @@
         <v>42701</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" si="1"/>
@@ -1808,9 +1775,9 @@
         <v>42702</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" si="1"/>
@@ -1824,7 +1791,7 @@
         <v>42707</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1840,9 +1807,9 @@
         <v>42709</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" si="1"/>
@@ -1856,9 +1823,9 @@
         <v>42717</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" si="1"/>
@@ -1872,7 +1839,10 @@
         <v>42731</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
       <c r="B17" s="2">
         <f t="shared" si="1"/>
         <v>42731</v>
@@ -1885,7 +1855,10 @@
         <v>42747</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
       <c r="B18" s="2">
         <f t="shared" si="1"/>
         <v>42747</v>
@@ -1898,7 +1871,10 @@
         <v>42752</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
       <c r="B19" s="2">
         <f t="shared" si="1"/>
         <v>42752</v>
@@ -1911,7 +1887,10 @@
         <v>42766</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
       <c r="B20" s="2">
         <f t="shared" si="1"/>
         <v>42766</v>
@@ -1924,9 +1903,9 @@
         <v>42773</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B21" s="2">
         <f t="shared" si="1"/>
@@ -1940,9 +1919,9 @@
         <v>42780</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B22" s="2">
         <f t="shared" si="1"/>
@@ -1956,51 +1935,8 @@
         <v>42794</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="2">
-        <f t="shared" si="1"/>
-        <v>42794</v>
-      </c>
-      <c r="C23">
-        <v>14</v>
-      </c>
-      <c r="D23" s="1">
-        <f t="shared" si="0"/>
-        <v>42808</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>16</v>
-      </c>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Connor: Updated Client UI to make it more uniform and updated documentation with meetings and notes on how to improve my solution approach/work plan/GanttChart
</commit_message>
<xml_diff>
--- a/Documentation/GanttChart.xlsx
+++ b/Documentation/GanttChart.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>TASK</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>Create Data Centre program to return web responses</t>
+  </si>
+  <si>
+    <t>Research efficient way to handle Edge Node resources</t>
+  </si>
+  <si>
+    <t>Implement Edge Node resource handling</t>
   </si>
 </sst>
 </file>
@@ -204,9 +210,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Gantt Chart'!$A$2:$A$22</c:f>
+              <c:f>'Gantt Chart'!$A$2:$A$24</c:f>
               <c:strCache>
-                <c:ptCount val="21"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>Buy and assemble componenets of the System</c:v>
                 </c:pt>
@@ -269,16 +275,22 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>Perform analysis and update machine learning application</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Research efficient way to handle Edge Node resources</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Implement Edge Node resource handling</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Gantt Chart'!$B$2:$B$22</c:f>
+              <c:f>'Gantt Chart'!$B$2:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>d/m;@</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>42654</c:v>
                 </c:pt>
@@ -307,40 +319,46 @@
                   <c:v>42694</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42699</c:v>
+                  <c:v>42701</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42701</c:v>
+                  <c:v>42703</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42702</c:v>
+                  <c:v>42704</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>42707</c:v>
+                  <c:v>42709</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>42709</c:v>
+                  <c:v>42716</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>42717</c:v>
+                  <c:v>42723</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>42731</c:v>
+                  <c:v>42737</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>42747</c:v>
+                  <c:v>42744</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>42752</c:v>
+                  <c:v>42751</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>42766</c:v>
+                  <c:v>42765</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>42773</c:v>
+                  <c:v>42781</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>42780</c:v>
+                  <c:v>42788</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>42802</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>42816</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -377,9 +395,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Gantt Chart'!$A$2:$A$22</c:f>
+              <c:f>'Gantt Chart'!$A$2:$A$24</c:f>
               <c:strCache>
-                <c:ptCount val="21"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>Buy and assemble componenets of the System</c:v>
                 </c:pt>
@@ -442,16 +460,22 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>Perform analysis and update machine learning application</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Research efficient way to handle Edge Node resources</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Implement Edge Node resource handling</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Gantt Chart'!$C$2:$C$22</c:f>
+              <c:f>'Gantt Chart'!$C$2:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -477,7 +501,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2</c:v>
@@ -489,30 +513,36 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
@@ -1574,19 +1604,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X30" sqref="X30"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="53.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1600,7 +1631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1615,7 +1646,7 @@
         <v>42659</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1627,16 +1658,16 @@
         <v>7</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D22" si="0">B3+C3</f>
+        <f t="shared" ref="D3:D24" si="0">B3+C3</f>
         <v>42666</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="2">
-        <f t="shared" ref="B4:B22" si="1">D3</f>
+        <f t="shared" ref="B4:B24" si="1">D3</f>
         <v>42666</v>
       </c>
       <c r="C4">
@@ -1647,7 +1678,7 @@
         <v>42670</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1663,7 +1694,7 @@
         <v>42676</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1679,7 +1710,7 @@
         <v>42680</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1695,7 +1726,7 @@
         <v>42686</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1711,7 +1742,7 @@
         <v>42688</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1727,7 +1758,7 @@
         <v>42694</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1736,207 +1767,236 @@
         <v>42694</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>42699</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42701</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" si="1"/>
-        <v>42699</v>
+        <v>42701</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>42701</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42703</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" si="1"/>
-        <v>42701</v>
+        <v>42703</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>42702</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42704</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" si="1"/>
-        <v>42702</v>
+        <v>42704</v>
       </c>
       <c r="C13">
         <v>5</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>42707</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42709</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" si="1"/>
-        <v>42707</v>
+        <v>42709</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>42709</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42716</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" si="1"/>
-        <v>42709</v>
+        <v>42716</v>
       </c>
       <c r="C15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>42717</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42723</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" si="1"/>
-        <v>42717</v>
+        <v>42723</v>
       </c>
       <c r="C16">
         <v>14</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
-        <v>42731</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42737</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" si="1"/>
-        <v>42731</v>
+        <v>42737</v>
       </c>
       <c r="C17">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="0"/>
-        <v>42747</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42744</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="2">
         <f t="shared" si="1"/>
-        <v>42747</v>
+        <v>42744</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="0"/>
-        <v>42752</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42751</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="2">
         <f t="shared" si="1"/>
-        <v>42752</v>
+        <v>42751</v>
       </c>
       <c r="C19">
         <v>14</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" si="0"/>
-        <v>42766</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42765</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" si="1"/>
-        <v>42766</v>
+        <v>42765</v>
       </c>
       <c r="C20">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="0"/>
-        <v>42773</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42781</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>14</v>
       </c>
       <c r="B21" s="2">
         <f t="shared" si="1"/>
-        <v>42773</v>
+        <v>42781</v>
       </c>
       <c r="C21">
         <v>7</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" si="0"/>
-        <v>42780</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42788</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="2">
         <f t="shared" si="1"/>
-        <v>42780</v>
+        <v>42788</v>
       </c>
       <c r="C22">
         <v>14</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" si="0"/>
-        <v>42794</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D23" s="1"/>
+        <v>42802</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="2">
+        <f t="shared" si="1"/>
+        <v>42802</v>
+      </c>
+      <c r="C23">
+        <v>14</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>42816</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="2">
+        <f t="shared" si="1"/>
+        <v>42816</v>
+      </c>
+      <c r="C24">
+        <v>14</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>42830</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Connor: Added updated files from yesterday for the example Nodejs container and the raw container files for a caching application in preparation for implementing a caching engine. Have done more research and got a private repository implemented. Also updated my Project description, solution approach and work plan and have submitted it for further review.
</commit_message>
<xml_diff>
--- a/Documentation/GanttChart.xlsx
+++ b/Documentation/GanttChart.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>TASK</t>
   </si>
@@ -41,22 +41,7 @@
     <t>Setup infrastructure to allow for deployment of applications</t>
   </si>
   <si>
-    <t>Create image for the cachine application</t>
-  </si>
-  <si>
     <t>Buy and assemble componenets of the System</t>
-  </si>
-  <si>
-    <t>Update Client Program to handle responses</t>
-  </si>
-  <si>
-    <t>Update Client Program to make multiple web requests</t>
-  </si>
-  <si>
-    <t>Research and design voice recognition application</t>
-  </si>
-  <si>
-    <t>Create image for voice recognition application</t>
   </si>
   <si>
     <t>Perform analysis and update caching application</t>
@@ -65,46 +50,28 @@
     <t>Perform analysis and update voice recognition application</t>
   </si>
   <si>
-    <t>Research and design machine learning application</t>
-  </si>
-  <si>
-    <t>Create image for machine learning application</t>
-  </si>
-  <si>
     <t>Perform analysis and update machine learning application</t>
   </si>
   <si>
-    <t>Update Data Centre program to process web requests</t>
+    <t>Create Client Application</t>
   </si>
   <si>
-    <t xml:space="preserve">Research and design caching application </t>
+    <t>Create Data Centre Application</t>
   </si>
   <si>
-    <t>Update Client Program Design</t>
+    <t>Create Edge Node Application</t>
   </si>
   <si>
-    <t>Update Data Centre Program to receive web requests</t>
+    <t xml:space="preserve">Research/design/create caching application </t>
   </si>
   <si>
-    <t>Update Edge Server Program to receive web requests</t>
+    <t>Research/design/create voice recognition application</t>
   </si>
   <si>
-    <t>Update Edge Server Program to process web requests</t>
+    <t>Research/design/create machine learning application</t>
   </si>
   <si>
-    <t>Create Basic Client Program to make web requests</t>
-  </si>
-  <si>
-    <t>Create Basic Edge Server Program to return web response</t>
-  </si>
-  <si>
-    <t>Create Data Centre program to return web responses</t>
-  </si>
-  <si>
-    <t>Research efficient way to handle Edge Node resources</t>
-  </si>
-  <si>
-    <t>Implement Edge Node resource handling</t>
+    <t>Research and implement efficient way to handle Edge Node resources</t>
   </si>
 </sst>
 </file>
@@ -210,9 +177,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Gantt Chart'!$A$2:$A$24</c:f>
+              <c:f>'Gantt Chart'!$A$2:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="23"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>Buy and assemble componenets of the System</c:v>
                 </c:pt>
@@ -220,77 +187,44 @@
                   <c:v>Setup infrastructure to allow for deployment of applications</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Create Basic Client Program to make web requests</c:v>
+                  <c:v>Create Edge Node Application</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Create Basic Edge Server Program to return web response</c:v>
+                  <c:v>Create Data Centre Application</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Create Data Centre program to return web responses</c:v>
+                  <c:v>Create Client Application</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Update Client Program Design</c:v>
+                  <c:v>Research/design/create caching application </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Update Edge Server Program to receive web requests</c:v>
+                  <c:v>Research/design/create voice recognition application</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Update Edge Server Program to process web requests</c:v>
+                  <c:v>Research/design/create machine learning application</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Update Data Centre Program to receive web requests</c:v>
+                  <c:v>Perform analysis and update caching application</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Update Data Centre program to process web requests</c:v>
+                  <c:v>Perform analysis and update voice recognition application</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Update Client Program to handle responses</c:v>
+                  <c:v>Perform analysis and update machine learning application</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Update Client Program to make multiple web requests</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Research and design caching application </c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Create image for the cachine application</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Perform analysis and update caching application</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Research and design voice recognition application</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Create image for voice recognition application</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Perform analysis and update voice recognition application</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Research and design machine learning application</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Create image for machine learning application</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Perform analysis and update machine learning application</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Research efficient way to handle Edge Node resources</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Implement Edge Node resource handling</c:v>
+                  <c:v>Research and implement efficient way to handle Edge Node resources</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Gantt Chart'!$B$2:$B$24</c:f>
+              <c:f>'Gantt Chart'!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>d/m;@</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>42654</c:v>
                 </c:pt>
@@ -301,64 +235,31 @@
                   <c:v>42666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42670</c:v>
+                  <c:v>42675</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42676</c:v>
+                  <c:v>42673</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42680</c:v>
+                  <c:v>42692</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42686</c:v>
+                  <c:v>42716</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42688</c:v>
+                  <c:v>42746</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42694</c:v>
+                  <c:v>42796</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42701</c:v>
+                  <c:v>42803</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42703</c:v>
+                  <c:v>42810</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42704</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>42709</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>42716</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>42723</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>42737</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>42744</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>42751</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>42765</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>42781</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>42788</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>42802</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>42816</c:v>
+                  <c:v>42817</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -395,9 +296,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Gantt Chart'!$A$2:$A$24</c:f>
+              <c:f>'Gantt Chart'!$A$2:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="23"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>Buy and assemble componenets of the System</c:v>
                 </c:pt>
@@ -405,77 +306,44 @@
                   <c:v>Setup infrastructure to allow for deployment of applications</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Create Basic Client Program to make web requests</c:v>
+                  <c:v>Create Edge Node Application</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Create Basic Edge Server Program to return web response</c:v>
+                  <c:v>Create Data Centre Application</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Create Data Centre program to return web responses</c:v>
+                  <c:v>Create Client Application</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Update Client Program Design</c:v>
+                  <c:v>Research/design/create caching application </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Update Edge Server Program to receive web requests</c:v>
+                  <c:v>Research/design/create voice recognition application</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Update Edge Server Program to process web requests</c:v>
+                  <c:v>Research/design/create machine learning application</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Update Data Centre Program to receive web requests</c:v>
+                  <c:v>Perform analysis and update caching application</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Update Data Centre program to process web requests</c:v>
+                  <c:v>Perform analysis and update voice recognition application</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Update Client Program to handle responses</c:v>
+                  <c:v>Perform analysis and update machine learning application</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Update Client Program to make multiple web requests</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Research and design caching application </c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Create image for the cachine application</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Perform analysis and update caching application</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Research and design voice recognition application</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Create image for voice recognition application</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Perform analysis and update voice recognition application</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Research and design machine learning application</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Create image for machine learning application</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Perform analysis and update machine learning application</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Research efficient way to handle Edge Node resources</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Implement Edge Node resource handling</c:v>
+                  <c:v>Research and implement efficient way to handle Edge Node resources</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Gantt Chart'!$C$2:$C$24</c:f>
+              <c:f>'Gantt Chart'!$C$2:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -483,66 +351,33 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="22">
                   <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
@@ -1607,17 +1442,17 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1631,9 +1466,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2">
         <v>42654</v>
@@ -1646,7 +1481,7 @@
         <v>42659</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1662,341 +1497,195 @@
         <v>42666</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2">
         <f t="shared" ref="B4:B24" si="1">D3</f>
         <v>42666</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>42670</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42687</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2">
-        <f t="shared" si="1"/>
-        <v>42670</v>
+        <v>42675</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>42676</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42688</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2">
+        <v>42673</v>
+      </c>
+      <c r="C6">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1">
+        <f>B6+C6</f>
+        <v>42692</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2">
+        <v>42692</v>
+      </c>
+      <c r="C7">
         <v>24</v>
-      </c>
-      <c r="B6" s="2">
-        <f t="shared" si="1"/>
-        <v>42676</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1">
-        <f t="shared" si="0"/>
-        <v>42680</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2">
-        <f t="shared" si="1"/>
-        <v>42680</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>42686</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42716</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" si="1"/>
-        <v>42686</v>
+        <v>42716</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>42688</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42746</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2">
-        <f t="shared" si="1"/>
-        <v>42688</v>
+        <f>D8</f>
+        <v>42746</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>42694</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42796</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" si="1"/>
-        <v>42694</v>
+        <v>42796</v>
       </c>
       <c r="C10">
         <v>7</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>42701</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42803</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" si="1"/>
-        <v>42701</v>
+        <v>42803</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>42703</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42810</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" si="1"/>
-        <v>42703</v>
+        <v>42810</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>42704</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42817</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" si="1"/>
-        <v>42704</v>
+        <v>42817</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>42709</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="2">
-        <f t="shared" si="1"/>
-        <v>42709</v>
-      </c>
-      <c r="C14">
-        <v>7</v>
-      </c>
-      <c r="D14" s="1">
-        <f t="shared" si="0"/>
-        <v>42716</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="2">
-        <f t="shared" si="1"/>
-        <v>42716</v>
-      </c>
-      <c r="C15">
-        <v>7</v>
-      </c>
-      <c r="D15" s="1">
-        <f t="shared" si="0"/>
-        <v>42723</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="2">
-        <f t="shared" si="1"/>
-        <v>42723</v>
-      </c>
-      <c r="C16">
-        <v>14</v>
-      </c>
-      <c r="D16" s="1">
-        <f t="shared" si="0"/>
-        <v>42737</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="2">
-        <f t="shared" si="1"/>
-        <v>42737</v>
-      </c>
-      <c r="C17">
-        <v>7</v>
-      </c>
-      <c r="D17" s="1">
-        <f t="shared" si="0"/>
-        <v>42744</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="2">
-        <f t="shared" si="1"/>
-        <v>42744</v>
-      </c>
-      <c r="C18">
-        <v>7</v>
-      </c>
-      <c r="D18" s="1">
-        <f t="shared" si="0"/>
-        <v>42751</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="2">
-        <f t="shared" si="1"/>
-        <v>42751</v>
-      </c>
-      <c r="C19">
-        <v>14</v>
-      </c>
-      <c r="D19" s="1">
-        <f t="shared" si="0"/>
-        <v>42765</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="2">
-        <f t="shared" si="1"/>
-        <v>42765</v>
-      </c>
-      <c r="C20">
-        <v>16</v>
-      </c>
-      <c r="D20" s="1">
-        <f t="shared" si="0"/>
-        <v>42781</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="2">
-        <f t="shared" si="1"/>
-        <v>42781</v>
-      </c>
-      <c r="C21">
-        <v>7</v>
-      </c>
-      <c r="D21" s="1">
-        <f t="shared" si="0"/>
-        <v>42788</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="2">
-        <f t="shared" si="1"/>
-        <v>42788</v>
-      </c>
-      <c r="C22">
-        <v>14</v>
-      </c>
-      <c r="D22" s="1">
-        <f t="shared" si="0"/>
-        <v>42802</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="2">
-        <f t="shared" si="1"/>
-        <v>42802</v>
-      </c>
-      <c r="C23">
-        <v>14</v>
-      </c>
-      <c r="D23" s="1">
-        <f t="shared" si="0"/>
-        <v>42816</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="2">
-        <f t="shared" si="1"/>
-        <v>42816</v>
-      </c>
-      <c r="C24">
-        <v>14</v>
-      </c>
-      <c r="D24" s="1">
-        <f t="shared" si="0"/>
-        <v>42830</v>
-      </c>
+        <v>42831</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>